<commit_message>
fix some bugs, and begin testing!
</commit_message>
<xml_diff>
--- a/kClist/Result/result.xlsx
+++ b/kClist/Result/result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gawssin\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F8B1A52A-70D6-497B-8DA3-D631589BEBBD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F3CE52FE-FD0D-46B0-B62B-22AC972D34F2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" xr2:uid="{B057552F-D38C-4CD0-B264-0A4C8ED1EFE9}"/>
   </bookViews>
@@ -25,16 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="40">
   <si>
     <t>k value</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1m24s</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1m48s</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -79,10 +75,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>8m53s</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>as-skitter, 24 threads</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -91,27 +83,107 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1m7s</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>result</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>7m43s</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11m39s</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1m22s</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>9m13s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>out.com-dblp, 24 threads</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1m21s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>21s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2m43s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2m23s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2m29s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2m35s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>23s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>14m27s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>34m58s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16m3s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>21m54s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>31m31s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3m42s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>out.orkut-links, 24 threads</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>55s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>39m32s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>22m4s</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -158,9 +230,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -482,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86605410-D1C4-4133-8024-3DB868ED9969}">
-  <dimension ref="A1:Q8"/>
+  <dimension ref="A1:Q35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -499,98 +574,134 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
+      <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1">
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="F2" s="1">
         <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="I2" s="1">
         <v>2</v>
       </c>
       <c r="J2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="L2" s="1">
         <v>3</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O2" s="1">
         <v>4</v>
       </c>
       <c r="P2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>3</v>
       </c>
+      <c r="B3" s="1">
+        <v>28769868</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>4</v>
       </c>
+      <c r="B4" s="1">
+        <v>148834439</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>5</v>
       </c>
+      <c r="B5" s="1">
+        <v>1183885507</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>6</v>
       </c>
+      <c r="B6" s="1">
+        <v>9759000981</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
@@ -600,19 +711,16 @@
         <v>73142566591</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="P7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
@@ -623,24 +731,520 @@
         <v>481576204696</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="P8" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2781731674867</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I15" s="2">
+        <v>2</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L15" s="2">
+        <v>3</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="O15" s="2">
+        <v>4</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q15" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>3</v>
+      </c>
+      <c r="B16" s="2">
+        <v>2224385</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>4</v>
+      </c>
+      <c r="B17" s="2">
+        <v>16713192</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>5</v>
+      </c>
+      <c r="B18" s="2">
+        <v>262663639</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>6</v>
+      </c>
+      <c r="B19" s="2">
+        <v>4221802226</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>7</v>
+      </c>
+      <c r="B20" s="2">
+        <v>60913718813</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>8</v>
+      </c>
+      <c r="B21" s="2">
+        <v>777232734905</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>9</v>
+      </c>
+      <c r="B22" s="1">
+        <v>8813264533265</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F28" s="2">
+        <v>1</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I28" s="2">
+        <v>2</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L28" s="2">
+        <v>3</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="O28" s="2">
+        <v>4</v>
+      </c>
+      <c r="P28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q28" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
+        <v>3</v>
+      </c>
+      <c r="B29" s="2">
+        <v>627577371</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
+        <v>4</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A31" s="2">
+        <v>5</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
+        <v>6</v>
+      </c>
+      <c r="B32" s="2">
+        <v>75233426735</v>
+      </c>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2"/>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A33" s="2">
+        <v>7</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A34" s="2">
+        <v>8</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A35" s="2">
+        <v>9</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+      <c r="P35" s="2"/>
+      <c r="Q35" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="A14:Q14"/>
+    <mergeCell ref="A27:Q27"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>